<commit_message>
checkpoint da automação das figuras do grupo 13
</commit_message>
<xml_diff>
--- a/Data/g13.1a.xlsx
+++ b/Data/g13.1a.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,14 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Região</t>
@@ -370,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Trimestre</t>
+          <t>Trimesetre</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -392,7 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -400,8 +476,8 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D2">
-        <v>56.37035083091533</v>
+      <c r="D2" t="n">
+        <v>56.37</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -417,7 +493,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -425,8 +501,8 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D3">
-        <v>55.26409595101801</v>
+      <c r="D3" t="n">
+        <v>55.26</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -442,7 +518,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -450,8 +526,8 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D4">
-        <v>54.49565798263193</v>
+      <c r="D4" t="n">
+        <v>54.5</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -467,7 +543,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -475,8 +551,8 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D5">
-        <v>54.4818048232345</v>
+      <c r="D5" t="n">
+        <v>54.48</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -492,7 +568,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -500,8 +576,8 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D6">
-        <v>54.41783649876135</v>
+      <c r="D6" t="n">
+        <v>54.42</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -517,7 +593,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -525,8 +601,8 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D7">
-        <v>54.28482393268931</v>
+      <c r="D7" t="n">
+        <v>54.28</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -542,7 +618,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -550,8 +626,8 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D8">
-        <v>46.78631051752922</v>
+      <c r="D8" t="n">
+        <v>46.79</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -562,12 +638,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -575,19 +651,20 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D9">
-        <v>43.92015762871584</v>
-      </c>
+      <c r="D9" t="n">
+        <v>50.67</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+          <t>Pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -595,11 +672,12 @@
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D10">
-        <v>50.66514405698735</v>
-      </c>
+      <c r="D10" t="n">
+        <v>43.92</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização das bases do grupo 13
</commit_message>
<xml_diff>
--- a/Data/g13.1a.xlsx
+++ b/Data/g13.1a.xlsx
@@ -473,11 +473,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>56.37</v>
+        <v>56.02</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -498,11 +498,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>55.26</v>
+        <v>55.75</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -513,7 +513,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Goiás</t>
+          <t>Rio Grande do Sul</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -523,11 +523,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>54.5</v>
+        <v>54.98</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -538,7 +538,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rio Grande do Sul</t>
+          <t>Distrito Federal</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -548,11 +548,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>54.48</v>
+        <v>54.88</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -573,11 +573,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>54.42</v>
+        <v>54.5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -588,7 +588,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Distrito Federal</t>
+          <t>Goiás</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -598,11 +598,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>54.28</v>
+        <v>54.02</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -623,15 +623,15 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>46.79</v>
+        <v>46.4</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>17º</t>
+          <t>18º</t>
         </is>
       </c>
     </row>
@@ -648,11 +648,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>50.67</v>
+        <v>50.87</v>
       </c>
       <c r="E9" t="inlineStr"/>
     </row>
@@ -669,11 +669,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>43.92</v>
+        <v>44.25</v>
       </c>
       <c r="E10" t="inlineStr"/>
     </row>

</xml_diff>